<commit_message>
FIX: PI3 diagrams editted
</commit_message>
<xml_diff>
--- a/datos_sms.xlsx
+++ b/datos_sms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\UNIR\Trabajo Fin de Master\Datos\qNLP-SMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED23FC4-8A0E-44D1-910E-6F68C4750427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBA0A18-8E03-4321-BAAC-345FA9B28DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejecución" sheetId="1" r:id="rId1"/>
@@ -2673,8 +2673,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2724,46 +2745,13 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2778,7 +2766,19 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4286,17 +4286,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Respuestas!$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Num</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4309,9 +4298,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Respuestas!$J$4:$J$12</c:f>
+              <c:f>Respuestas!$J$4:$J$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>english</c:v>
                 </c:pt>
@@ -4339,15 +4328,18 @@
                 <c:pt idx="8">
                   <c:v>mof description</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>c/c++</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Respuestas!$K$4:$K$12</c:f>
+              <c:f>Respuestas!$K$4:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>108</c:v>
                 </c:pt>
@@ -4373,6 +4365,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -4667,7 +4662,7 @@
                   <c:v>hindi</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ns</c:v>
+                  <c:v>indefinido</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>musical</c:v>
@@ -4994,7 +4989,7 @@
                   <c:v>english</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ns</c:v>
+                  <c:v>indefinido</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>formal language</c:v>
@@ -9101,38 +9096,38 @@
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="70" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="68"/>
+      <c r="B2" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
       <c r="H2" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="68"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -9149,7 +9144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -9169,7 +9164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -9186,7 +9181,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -9203,18 +9198,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="58">
         <v>1393</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -9248,35 +9243,35 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="62" t="s">
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="72" t="s">
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="70"/>
+      <c r="B12" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
       <c r="G12" s="13"/>
       <c r="H12" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="70"/>
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -9297,7 +9292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -9319,7 +9314,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -9340,7 +9335,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
@@ -9361,22 +9356,22 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="58">
         <v>600</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
@@ -9397,7 +9392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
@@ -9418,46 +9413,46 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="60"/>
       <c r="F20" s="17">
         <f>SUM(F14:F19)</f>
         <v>2803</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="66" t="s">
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A22" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
-      <c r="B23" s="78" t="s">
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="74"/>
+      <c r="B23" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
       <c r="H23" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="67"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="74"/>
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
@@ -9477,7 +9472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>4</v>
       </c>
@@ -9501,7 +9496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>5</v>
       </c>
@@ -9525,7 +9520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>6</v>
       </c>
@@ -9546,22 +9541,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="56">
+      <c r="B28" s="58">
         <v>65</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="21">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>8</v>
       </c>
@@ -9582,7 +9577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>9</v>
       </c>
@@ -9603,46 +9598,46 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="16"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="79" t="s">
+      <c r="D31" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="79"/>
+      <c r="E31" s="63"/>
       <c r="F31" s="22">
         <f>SUM(F25:F30)</f>
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="68" t="s">
+    <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A33" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="73"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="74" t="s">
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="76"/>
+      <c r="B34" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
       <c r="H34" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="76"/>
       <c r="B35" s="10" t="s">
         <v>0</v>
       </c>
@@ -9662,7 +9657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>4</v>
       </c>
@@ -9686,7 +9681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>5</v>
       </c>
@@ -9707,7 +9702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>6</v>
       </c>
@@ -9728,22 +9723,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="56">
+      <c r="B39" s="58">
         <v>65</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="25">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>8</v>
       </c>
@@ -9764,7 +9759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>9</v>
       </c>
@@ -9785,76 +9780,68 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D42" s="71" t="s">
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="D42" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="E42" s="71"/>
+      <c r="E42" s="78"/>
       <c r="F42" s="26">
         <f>SUM(F36:F41)</f>
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A44" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
       <c r="H44" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65" t="s">
+      <c r="C45" s="72"/>
+      <c r="D45" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
       <c r="H45" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>112</v>
       </c>
-      <c r="B46" s="56">
+      <c r="B46" s="58">
         <v>48</v>
       </c>
-      <c r="C46" s="56"/>
-      <c r="D46" s="57">
+      <c r="C46" s="58"/>
+      <c r="D46" s="64">
         <f>SUM(A46:C46)</f>
         <v>160</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
       <c r="H46" s="4" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D31:E31"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D46:F46"/>
     <mergeCell ref="B1:E1"/>
@@ -9871,6 +9858,14 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9880,26 +9875,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728319D4-8A53-4E77-BB8C-AB333061B314}">
   <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="33" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="33" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="33" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="118.5703125" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="11.5703125" style="32"/>
+    <col min="1" max="1" width="7.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="33" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="33" customWidth="1"/>
+    <col min="10" max="10" width="118.5546875" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>43</v>
       </c>
@@ -9931,7 +9926,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>44</v>
       </c>
@@ -9960,7 +9955,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>52</v>
       </c>
@@ -9992,7 +9987,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>88</v>
       </c>
@@ -10021,7 +10016,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>89</v>
       </c>
@@ -10050,7 +10045,7 @@
         <v>44866</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>90</v>
       </c>
@@ -10079,7 +10074,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>91</v>
       </c>
@@ -10108,7 +10103,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>92</v>
       </c>
@@ -10137,7 +10132,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>93</v>
       </c>
@@ -10169,7 +10164,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>94</v>
       </c>
@@ -10201,7 +10196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>95</v>
       </c>
@@ -10233,7 +10228,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>96</v>
       </c>
@@ -10265,7 +10260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>97</v>
       </c>
@@ -10294,7 +10289,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>98</v>
       </c>
@@ -10326,7 +10321,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>99</v>
       </c>
@@ -10358,7 +10353,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>100</v>
       </c>
@@ -10387,7 +10382,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>115</v>
       </c>
@@ -10419,7 +10414,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>116</v>
       </c>
@@ -10448,7 +10443,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>117</v>
       </c>
@@ -10480,7 +10475,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>118</v>
       </c>
@@ -10512,7 +10507,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>119</v>
       </c>
@@ -10544,7 +10539,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="33" t="s">
         <v>139</v>
       </c>
@@ -10576,7 +10571,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
         <v>140</v>
       </c>
@@ -10608,7 +10603,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
         <v>141</v>
       </c>
@@ -10637,7 +10632,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
         <v>142</v>
       </c>
@@ -10666,7 +10661,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
         <v>143</v>
       </c>
@@ -10695,7 +10690,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>144</v>
       </c>
@@ -10727,7 +10722,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
         <v>145</v>
       </c>
@@ -10759,7 +10754,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>146</v>
       </c>
@@ -10791,7 +10786,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
         <v>147</v>
       </c>
@@ -10823,7 +10818,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
         <v>153</v>
       </c>
@@ -10855,7 +10850,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
         <v>160</v>
       </c>
@@ -10884,7 +10879,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>161</v>
       </c>
@@ -10916,7 +10911,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="33" t="s">
         <v>162</v>
       </c>
@@ -10948,7 +10943,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
         <v>163</v>
       </c>
@@ -10980,7 +10975,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="33" t="s">
         <v>164</v>
       </c>
@@ -11012,7 +11007,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
         <v>196</v>
       </c>
@@ -11041,7 +11036,7 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
         <v>197</v>
       </c>
@@ -11070,7 +11065,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
         <v>198</v>
       </c>
@@ -11099,7 +11094,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
         <v>199</v>
       </c>
@@ -11131,7 +11126,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="33" t="s">
         <v>200</v>
       </c>
@@ -11163,7 +11158,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
         <v>201</v>
       </c>
@@ -11192,7 +11187,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
         <v>202</v>
       </c>
@@ -11221,7 +11216,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>203</v>
       </c>
@@ -11253,7 +11248,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>204</v>
       </c>
@@ -11285,7 +11280,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>211</v>
       </c>
@@ -11314,7 +11309,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>212</v>
       </c>
@@ -11343,7 +11338,7 @@
         <v>45505</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>213</v>
       </c>
@@ -11375,7 +11370,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>214</v>
       </c>
@@ -11404,7 +11399,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
         <v>215</v>
       </c>
@@ -11433,7 +11428,7 @@
         <v>44593</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
         <v>225</v>
       </c>
@@ -11465,7 +11460,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
         <v>242</v>
       </c>
@@ -11497,7 +11492,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
         <v>243</v>
       </c>
@@ -11526,7 +11521,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>244</v>
       </c>
@@ -11555,7 +11550,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
         <v>245</v>
       </c>
@@ -11587,7 +11582,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="33" t="s">
         <v>246</v>
       </c>
@@ -11619,7 +11614,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
         <v>247</v>
       </c>
@@ -11648,7 +11643,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="33" t="s">
         <v>248</v>
       </c>
@@ -11677,7 +11672,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="33" t="s">
         <v>251</v>
       </c>
@@ -11706,7 +11701,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="33" t="s">
         <v>306</v>
       </c>
@@ -11738,7 +11733,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="33" t="s">
         <v>307</v>
       </c>
@@ -11767,7 +11762,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
         <v>308</v>
       </c>
@@ -11799,7 +11794,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
         <v>309</v>
       </c>
@@ -11828,7 +11823,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
         <v>310</v>
       </c>
@@ -11857,7 +11852,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
         <v>311</v>
       </c>
@@ -11889,7 +11884,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
         <v>312</v>
       </c>
@@ -11918,7 +11913,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
         <v>313</v>
       </c>
@@ -11947,7 +11942,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="33" t="s">
         <v>314</v>
       </c>
@@ -11976,7 +11971,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="33" t="s">
         <v>315</v>
       </c>
@@ -12005,7 +12000,7 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
         <v>316</v>
       </c>
@@ -12037,7 +12032,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="33" t="s">
         <v>317</v>
       </c>
@@ -12066,7 +12061,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
         <v>318</v>
       </c>
@@ -12095,7 +12090,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
         <v>319</v>
       </c>
@@ -12124,7 +12119,7 @@
         <v>44958</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="33" t="s">
         <v>320</v>
       </c>
@@ -12153,7 +12148,7 @@
         <v>44896</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
         <v>321</v>
       </c>
@@ -12182,7 +12177,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="33" t="s">
         <v>322</v>
       </c>
@@ -12211,7 +12206,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
         <v>323</v>
       </c>
@@ -12240,7 +12235,7 @@
         <v>45597</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>324</v>
       </c>
@@ -12269,7 +12264,7 @@
         <v>44075</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>333</v>
       </c>
@@ -12298,7 +12293,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>334</v>
       </c>
@@ -12330,7 +12325,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>335</v>
       </c>
@@ -12359,7 +12354,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>336</v>
       </c>
@@ -12388,7 +12383,7 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>340</v>
       </c>
@@ -12417,7 +12412,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
         <v>366</v>
       </c>
@@ -12446,7 +12441,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="33" t="s">
         <v>367</v>
       </c>
@@ -12478,7 +12473,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="33" t="s">
         <v>368</v>
       </c>
@@ -12507,7 +12502,7 @@
         <v>44835</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="33" t="s">
         <v>369</v>
       </c>
@@ -12536,7 +12531,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="33" t="s">
         <v>370</v>
       </c>
@@ -12565,7 +12560,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="33" t="s">
         <v>371</v>
       </c>
@@ -12594,7 +12589,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="33" t="s">
         <v>372</v>
       </c>
@@ -12626,7 +12621,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="33" t="s">
         <v>373</v>
       </c>
@@ -12655,7 +12650,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="33" t="s">
         <v>374</v>
       </c>
@@ -12684,7 +12679,7 @@
         <v>44348</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="33" t="s">
         <v>375</v>
       </c>
@@ -12713,7 +12708,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="33" t="s">
         <v>376</v>
       </c>
@@ -12742,7 +12737,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="33" t="s">
         <v>377</v>
       </c>
@@ -12771,7 +12766,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="33" t="s">
         <v>394</v>
       </c>
@@ -12800,7 +12795,7 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="33" t="s">
         <v>395</v>
       </c>
@@ -12829,7 +12824,7 @@
         <v>44470</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="33" t="s">
         <v>396</v>
       </c>
@@ -12858,7 +12853,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="33" t="s">
         <v>397</v>
       </c>
@@ -12887,7 +12882,7 @@
         <v>44621</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="33" t="s">
         <v>398</v>
       </c>
@@ -12916,7 +12911,7 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="33" t="s">
         <v>399</v>
       </c>
@@ -12945,7 +12940,7 @@
         <v>44501</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="33" t="s">
         <v>400</v>
       </c>
@@ -12974,7 +12969,7 @@
         <v>45383</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="33" t="s">
         <v>401</v>
       </c>
@@ -13003,7 +12998,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="33" t="s">
         <v>477</v>
       </c>
@@ -13032,7 +13027,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="33" t="s">
         <v>478</v>
       </c>
@@ -13064,7 +13059,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="33" t="s">
         <v>479</v>
       </c>
@@ -13096,7 +13091,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="33" t="s">
         <v>480</v>
       </c>
@@ -13125,7 +13120,7 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="33" t="s">
         <v>481</v>
       </c>
@@ -13154,7 +13149,7 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="33" t="s">
         <v>482</v>
       </c>
@@ -13183,7 +13178,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="33" t="s">
         <v>483</v>
       </c>
@@ -13212,7 +13207,7 @@
         <v>44593</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="33" t="s">
         <v>484</v>
       </c>
@@ -13241,7 +13236,7 @@
         <v>44621</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="33" t="s">
         <v>485</v>
       </c>
@@ -13273,7 +13268,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="33" t="s">
         <v>486</v>
       </c>
@@ -13302,7 +13297,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="33" t="s">
         <v>487</v>
       </c>
@@ -13331,7 +13326,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="33" t="s">
         <v>488</v>
       </c>
@@ -13360,7 +13355,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="33" t="s">
         <v>489</v>
       </c>
@@ -13389,7 +13384,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="33" t="s">
         <v>490</v>
       </c>
@@ -13418,7 +13413,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="33" t="s">
         <v>491</v>
       </c>
@@ -13447,7 +13442,7 @@
         <v>44348</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="33" t="s">
         <v>492</v>
       </c>
@@ -13476,7 +13471,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="33" t="s">
         <v>493</v>
       </c>
@@ -13505,7 +13500,7 @@
         <v>44866</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="33" t="s">
         <v>494</v>
       </c>
@@ -13534,7 +13529,7 @@
         <v>45383</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="33" t="s">
         <v>495</v>
       </c>
@@ -13563,7 +13558,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="33" t="s">
         <v>496</v>
       </c>
@@ -13592,7 +13587,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="33" t="s">
         <v>497</v>
       </c>
@@ -13621,7 +13616,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="33" t="s">
         <v>498</v>
       </c>
@@ -13650,7 +13645,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="33" t="s">
         <v>499</v>
       </c>
@@ -13679,7 +13674,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="33" t="s">
         <v>500</v>
       </c>
@@ -13708,7 +13703,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="33" t="s">
         <v>501</v>
       </c>
@@ -13737,7 +13732,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" s="33" t="s">
         <v>502</v>
       </c>
@@ -13766,7 +13761,7 @@
         <v>44866</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="33" t="s">
         <v>503</v>
       </c>
@@ -13795,7 +13790,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="33" t="s">
         <v>504</v>
       </c>
@@ -13824,7 +13819,7 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="33" t="s">
         <v>505</v>
       </c>
@@ -13853,7 +13848,7 @@
         <v>44593</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="33" t="s">
         <v>506</v>
       </c>
@@ -13882,7 +13877,7 @@
         <v>44896</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="33" t="s">
         <v>507</v>
       </c>
@@ -13911,7 +13906,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="33" t="s">
         <v>508</v>
       </c>
@@ -13940,7 +13935,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="33" t="s">
         <v>509</v>
       </c>
@@ -13969,7 +13964,7 @@
         <v>45474</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="33" t="s">
         <v>531</v>
       </c>
@@ -13998,7 +13993,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="33" t="s">
         <v>532</v>
       </c>
@@ -14027,7 +14022,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="33" t="s">
         <v>533</v>
       </c>
@@ -14056,7 +14051,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="33" t="s">
         <v>534</v>
       </c>
@@ -14085,7 +14080,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="33" t="s">
         <v>535</v>
       </c>
@@ -14114,7 +14109,7 @@
         <v>45383</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="33" t="s">
         <v>536</v>
       </c>
@@ -14143,7 +14138,7 @@
         <v>44348</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="33" t="s">
         <v>537</v>
       </c>
@@ -14172,7 +14167,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="33" t="s">
         <v>538</v>
       </c>
@@ -14204,7 +14199,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="33" t="s">
         <v>539</v>
       </c>
@@ -14233,7 +14228,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="33" t="s">
         <v>540</v>
       </c>
@@ -14262,7 +14257,7 @@
         <v>44835</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="33" t="s">
         <v>541</v>
       </c>
@@ -14291,7 +14286,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="33" t="s">
         <v>542</v>
       </c>
@@ -14320,7 +14315,7 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="33" t="s">
         <v>543</v>
       </c>
@@ -14349,7 +14344,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="33" t="s">
         <v>544</v>
       </c>
@@ -14378,7 +14373,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="33" t="s">
         <v>545</v>
       </c>
@@ -14407,7 +14402,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="33" t="s">
         <v>546</v>
       </c>
@@ -14436,7 +14431,7 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="33" t="s">
         <v>547</v>
       </c>
@@ -14465,7 +14460,7 @@
         <v>44866</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="33" t="s">
         <v>548</v>
       </c>
@@ -14494,7 +14489,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="33" t="s">
         <v>560</v>
       </c>
@@ -14523,7 +14518,7 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="33" t="s">
         <v>564</v>
       </c>
@@ -14552,7 +14547,7 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="33" t="s">
         <v>568</v>
       </c>
@@ -14581,7 +14576,7 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="33" t="s">
         <v>571</v>
       </c>
@@ -14610,7 +14605,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="33" t="s">
         <v>572</v>
       </c>
@@ -14639,7 +14634,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="33" t="s">
         <v>576</v>
       </c>
@@ -14668,7 +14663,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="33" t="s">
         <v>577</v>
       </c>
@@ -14709,18 +14704,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4391A-086D-47C7-B013-B10367BD67F6}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" style="32" customWidth="1"/>
     <col min="2" max="2" width="173" style="32" customWidth="1"/>
-    <col min="3" max="16384" width="11.5703125" style="32"/>
+    <col min="3" max="16384" width="11.5546875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="36" t="s">
         <v>266</v>
       </c>
@@ -14728,7 +14723,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>123</v>
       </c>
@@ -14736,7 +14731,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>269</v>
       </c>
@@ -14744,7 +14739,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>222</v>
       </c>
@@ -14752,7 +14747,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>339</v>
       </c>
@@ -14760,7 +14755,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>387</v>
       </c>
@@ -14768,7 +14763,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>157</v>
       </c>
@@ -14776,7 +14771,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>37</v>
       </c>
@@ -14784,7 +14779,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>64</v>
       </c>
@@ -14792,7 +14787,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>264</v>
       </c>
@@ -14800,7 +14795,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>294</v>
       </c>
@@ -14808,7 +14803,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>298</v>
       </c>
@@ -14816,7 +14811,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>331</v>
       </c>
@@ -14824,7 +14819,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>352</v>
       </c>
@@ -14832,7 +14827,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>390</v>
       </c>
@@ -14840,7 +14835,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>428</v>
       </c>
@@ -14848,7 +14843,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>432</v>
       </c>
@@ -14856,7 +14851,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
         <v>439</v>
       </c>
@@ -14864,7 +14859,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>472</v>
       </c>
@@ -14872,7 +14867,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>475</v>
       </c>
@@ -14880,7 +14875,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>515</v>
       </c>
@@ -14888,7 +14883,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>522</v>
       </c>
@@ -14896,7 +14891,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>596</v>
       </c>
@@ -14913,112 +14908,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F3EEE0-596F-49A8-8C07-C0EC0504D81F}">
   <dimension ref="A1:Z139"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37:K47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" customWidth="1"/>
-    <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="5.109375" customWidth="1"/>
+    <col min="15" max="15" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="2.7109375" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" customWidth="1"/>
-    <col min="21" max="21" width="2.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" customWidth="1"/>
-    <col min="23" max="23" width="5.140625" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" customWidth="1"/>
-    <col min="26" max="26" width="5.85546875" customWidth="1"/>
+    <col min="18" max="18" width="2.6640625" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" customWidth="1"/>
+    <col min="21" max="21" width="2.6640625" customWidth="1"/>
+    <col min="22" max="22" width="12.109375" customWidth="1"/>
+    <col min="23" max="23" width="5.109375" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" customWidth="1"/>
+    <col min="26" max="26" width="5.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="90" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="G1" s="83" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="G1" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="83"/>
-      <c r="J1" s="84" t="s">
+      <c r="H1" s="91"/>
+      <c r="J1" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="M1" s="87" t="s">
+      <c r="K1" s="87"/>
+      <c r="M1" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="P1" s="88" t="s">
+      <c r="N1" s="83"/>
+      <c r="P1" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="V1" s="89" t="s">
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="V1" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
         <v>581</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="D2" s="81" t="s">
+      <c r="B2" s="89"/>
+      <c r="D2" s="89" t="s">
         <v>628</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="G2" s="80" t="s">
+      <c r="E2" s="89"/>
+      <c r="G2" s="88" t="s">
         <v>581</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="J2" s="85" t="s">
+      <c r="H2" s="88"/>
+      <c r="J2" s="80" t="s">
         <v>581</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="M2" s="90" t="s">
+      <c r="K2" s="80"/>
+      <c r="M2" s="86" t="s">
         <v>581</v>
       </c>
-      <c r="N2" s="90"/>
-      <c r="P2" s="91" t="s">
+      <c r="N2" s="86"/>
+      <c r="P2" s="82" t="s">
         <v>581</v>
       </c>
-      <c r="Q2" s="91"/>
-      <c r="S2" s="91" t="s">
+      <c r="Q2" s="82"/>
+      <c r="S2" s="82" t="s">
         <v>628</v>
       </c>
-      <c r="T2" s="91"/>
-      <c r="V2" s="86" t="s">
+      <c r="T2" s="82"/>
+      <c r="V2" s="81" t="s">
         <v>581</v>
       </c>
-      <c r="W2" s="86"/>
-      <c r="Y2" s="86" t="s">
+      <c r="W2" s="81"/>
+      <c r="Y2" s="81" t="s">
         <v>628</v>
       </c>
-      <c r="Z2" s="86"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z2" s="81"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>266</v>
       </c>
@@ -15074,7 +15069,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>583</v>
       </c>
@@ -15130,7 +15125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>585</v>
       </c>
@@ -15155,6 +15150,10 @@
       <c r="K5" s="41">
         <v>30</v>
       </c>
+      <c r="L5" s="42">
+        <f>K5/SUM(K4:K23)</f>
+        <v>0.17142857142857143</v>
+      </c>
       <c r="M5" s="11" t="s">
         <v>673</v>
       </c>
@@ -15186,7 +15185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>587</v>
       </c>
@@ -15242,7 +15241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>590</v>
       </c>
@@ -15298,7 +15297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>609</v>
       </c>
@@ -15354,7 +15353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>604</v>
       </c>
@@ -15410,7 +15409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>606</v>
       </c>
@@ -15466,7 +15465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>598</v>
       </c>
@@ -15522,7 +15521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>611</v>
       </c>
@@ -15574,7 +15573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>588</v>
       </c>
@@ -15587,10 +15586,10 @@
       <c r="E13" s="42">
         <v>4</v>
       </c>
-      <c r="G13" s="80" t="s">
+      <c r="G13" s="88" t="s">
         <v>629</v>
       </c>
-      <c r="H13" s="80"/>
+      <c r="H13" s="88"/>
       <c r="J13" s="52" t="s">
         <v>661</v>
       </c>
@@ -15624,7 +15623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>589</v>
       </c>
@@ -15650,10 +15649,10 @@
       <c r="K14" s="41">
         <v>2</v>
       </c>
-      <c r="M14" s="90" t="s">
+      <c r="M14" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="90"/>
+      <c r="N14" s="86"/>
       <c r="P14" s="55" t="s">
         <v>688</v>
       </c>
@@ -15674,7 +15673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>592</v>
       </c>
@@ -15713,22 +15712,22 @@
       <c r="W15" s="42">
         <v>5</v>
       </c>
-      <c r="Y15" s="86" t="s">
+      <c r="Y15" s="81" t="s">
         <v>629</v>
       </c>
-      <c r="Z15" s="86"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z15" s="81"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>602</v>
       </c>
       <c r="B16" s="43">
         <v>3</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="D16" s="89" t="s">
         <v>629</v>
       </c>
-      <c r="E16" s="81"/>
+      <c r="E16" s="89"/>
       <c r="G16" s="6" t="s">
         <v>641</v>
       </c>
@@ -15753,10 +15752,10 @@
       <c r="Q16" s="42">
         <v>3</v>
       </c>
-      <c r="S16" s="91" t="s">
+      <c r="S16" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="91"/>
+      <c r="T16" s="82"/>
       <c r="V16" s="48">
         <v>44958</v>
       </c>
@@ -15770,7 +15769,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>608</v>
       </c>
@@ -15826,7 +15825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>615</v>
       </c>
@@ -15878,7 +15877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>584</v>
       </c>
@@ -15891,10 +15890,10 @@
       <c r="E19" s="42">
         <v>19</v>
       </c>
-      <c r="G19" s="80" t="s">
+      <c r="G19" s="88" t="s">
         <v>630</v>
       </c>
-      <c r="H19" s="80"/>
+      <c r="H19" s="88"/>
       <c r="J19" s="52" t="s">
         <v>666</v>
       </c>
@@ -15932,7 +15931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>593</v>
       </c>
@@ -15988,7 +15987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>595</v>
       </c>
@@ -16040,7 +16039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>599</v>
       </c>
@@ -16065,10 +16064,10 @@
       <c r="K22" s="41">
         <v>1</v>
       </c>
-      <c r="M22" s="90" t="s">
+      <c r="M22" s="86" t="s">
         <v>582</v>
       </c>
-      <c r="N22" s="90"/>
+      <c r="N22" s="86"/>
       <c r="P22" s="55" t="s">
         <v>696</v>
       </c>
@@ -16094,7 +16093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>613</v>
       </c>
@@ -16150,7 +16149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>620</v>
       </c>
@@ -16170,7 +16169,6 @@
         <v>637</v>
       </c>
       <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
       <c r="M24" s="53" t="s">
         <v>672</v>
       </c>
@@ -16202,7 +16200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>586</v>
       </c>
@@ -16221,10 +16219,10 @@
       <c r="H25" s="42" t="s">
         <v>638</v>
       </c>
-      <c r="J25" s="85" t="s">
+      <c r="J25" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="85"/>
+      <c r="K25" s="80"/>
       <c r="M25" s="53" t="s">
         <v>674</v>
       </c>
@@ -16256,7 +16254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>591</v>
       </c>
@@ -16306,7 +16304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>594</v>
       </c>
@@ -16350,7 +16348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>596</v>
       </c>
@@ -16394,12 +16392,12 @@
       <c r="W28" s="42">
         <v>3</v>
       </c>
-      <c r="Y28" s="86" t="s">
+      <c r="Y28" s="81" t="s">
         <v>653</v>
       </c>
-      <c r="Z28" s="86"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z28" s="81"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>597</v>
       </c>
@@ -16441,17 +16439,17 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>600</v>
       </c>
       <c r="B30" s="43">
         <v>1</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="89" t="s">
         <v>630</v>
       </c>
-      <c r="E30" s="81"/>
+      <c r="E30" s="89"/>
       <c r="J30" s="52" t="s">
         <v>659</v>
       </c>
@@ -16470,10 +16468,10 @@
       <c r="Q30" s="42">
         <v>1</v>
       </c>
-      <c r="S30" s="91" t="s">
+      <c r="S30" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="T30" s="91"/>
+      <c r="T30" s="82"/>
       <c r="V30" s="48">
         <v>44774</v>
       </c>
@@ -16487,7 +16485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>601</v>
       </c>
@@ -16501,7 +16499,7 @@
         <v>580</v>
       </c>
       <c r="J31" s="52" t="s">
-        <v>590</v>
+        <v>625</v>
       </c>
       <c r="K31" s="41">
         <v>1</v>
@@ -16531,7 +16529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>603</v>
       </c>
@@ -16575,7 +16573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>605</v>
       </c>
@@ -16619,7 +16617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>607</v>
       </c>
@@ -16663,7 +16661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>610</v>
       </c>
@@ -16703,7 +16701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>612</v>
       </c>
@@ -16716,10 +16714,10 @@
       <c r="E36" s="43">
         <v>6</v>
       </c>
-      <c r="J36" s="85" t="s">
+      <c r="J36" s="80" t="s">
         <v>582</v>
       </c>
-      <c r="K36" s="85"/>
+      <c r="K36" s="80"/>
       <c r="P36" s="55" t="s">
         <v>711</v>
       </c>
@@ -16745,7 +16743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>614</v>
       </c>
@@ -16789,7 +16787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>616</v>
       </c>
@@ -16833,7 +16831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>617</v>
       </c>
@@ -16847,11 +16845,15 @@
         <v>5</v>
       </c>
       <c r="J39" s="52" t="s">
-        <v>590</v>
+        <v>625</v>
       </c>
       <c r="K39" s="41">
         <v>29</v>
       </c>
+      <c r="L39" s="39">
+        <f>K39/SUM(K38:K55)</f>
+        <v>0.23966942148760331</v>
+      </c>
       <c r="P39" s="55" t="s">
         <v>714</v>
       </c>
@@ -16877,7 +16879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>618</v>
       </c>
@@ -16911,7 +16913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>619</v>
       </c>
@@ -16930,10 +16932,10 @@
       <c r="K41" s="41">
         <v>4</v>
       </c>
-      <c r="P41" s="91" t="s">
+      <c r="P41" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="Q41" s="91"/>
+      <c r="Q41" s="82"/>
       <c r="S41" s="54" t="s">
         <v>695</v>
       </c>
@@ -16947,7 +16949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>621</v>
       </c>
@@ -16987,7 +16989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>622</v>
       </c>
@@ -17013,7 +17015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>623</v>
       </c>
@@ -17039,7 +17041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="41"/>
       <c r="B45" s="41"/>
       <c r="J45" s="52" t="s">
@@ -17061,11 +17063,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="81" t="s">
+    <row r="46" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="81"/>
+      <c r="B46" s="89"/>
       <c r="J46" s="52" t="s">
         <v>659</v>
       </c>
@@ -17085,7 +17087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="40" t="s">
         <v>266</v>
       </c>
@@ -17111,7 +17113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>585</v>
       </c>
@@ -17137,7 +17139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>583</v>
       </c>
@@ -17163,7 +17165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>587</v>
       </c>
@@ -17189,7 +17191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>584</v>
       </c>
@@ -17215,7 +17217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>588</v>
       </c>
@@ -17241,7 +17243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>590</v>
       </c>
@@ -17267,7 +17269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>586</v>
       </c>
@@ -17293,7 +17295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>589</v>
       </c>
@@ -17318,7 +17320,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>591</v>
       </c>
@@ -17334,7 +17336,7 @@
       <c r="V56" s="41"/>
       <c r="W56" s="41"/>
     </row>
-    <row r="57" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>592</v>
       </c>
@@ -17347,12 +17349,12 @@
       <c r="Q57" s="42">
         <v>1</v>
       </c>
-      <c r="V57" s="86" t="s">
+      <c r="V57" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="W57" s="86"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W57" s="81"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>593</v>
       </c>
@@ -17372,7 +17374,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="P59" s="54" t="s">
         <v>693</v>
       </c>
@@ -17386,11 +17388,11 @@
         <v>636</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="81" t="s">
+    <row r="60" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="89" t="s">
         <v>582</v>
       </c>
-      <c r="B60" s="81"/>
+      <c r="B60" s="89"/>
       <c r="P60" s="54" t="s">
         <v>705</v>
       </c>
@@ -17404,7 +17406,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="40" t="s">
         <v>266</v>
       </c>
@@ -17420,17 +17422,17 @@
         <v>636</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>583</v>
       </c>
       <c r="B62" s="43">
         <v>43</v>
       </c>
-      <c r="P62" s="91" t="s">
+      <c r="P62" s="82" t="s">
         <v>582</v>
       </c>
-      <c r="Q62" s="91"/>
+      <c r="Q62" s="82"/>
       <c r="V62" s="48">
         <v>45231</v>
       </c>
@@ -17438,7 +17440,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>587</v>
       </c>
@@ -17458,7 +17460,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>609</v>
       </c>
@@ -17478,7 +17480,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>625</v>
       </c>
@@ -17498,7 +17500,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>604</v>
       </c>
@@ -17518,7 +17520,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>606</v>
       </c>
@@ -17538,7 +17540,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>598</v>
       </c>
@@ -17558,7 +17560,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>611</v>
       </c>
@@ -17578,7 +17580,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>602</v>
       </c>
@@ -17598,7 +17600,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>608</v>
       </c>
@@ -17618,7 +17620,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>615</v>
       </c>
@@ -17638,7 +17640,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>595</v>
       </c>
@@ -17658,7 +17660,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>599</v>
       </c>
@@ -17678,7 +17680,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>589</v>
       </c>
@@ -17698,7 +17700,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>592</v>
       </c>
@@ -17718,7 +17720,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>588</v>
       </c>
@@ -17738,7 +17740,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>613</v>
       </c>
@@ -17758,7 +17760,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>620</v>
       </c>
@@ -17778,7 +17780,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>593</v>
       </c>
@@ -17798,7 +17800,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>594</v>
       </c>
@@ -17818,7 +17820,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>596</v>
       </c>
@@ -17838,7 +17840,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>597</v>
       </c>
@@ -17858,7 +17860,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>600</v>
       </c>
@@ -17878,7 +17880,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>601</v>
       </c>
@@ -17898,7 +17900,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>603</v>
       </c>
@@ -17918,7 +17920,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>605</v>
       </c>
@@ -17938,7 +17940,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>607</v>
       </c>
@@ -17958,7 +17960,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>610</v>
       </c>
@@ -17974,7 +17976,7 @@
       <c r="V89" s="41"/>
       <c r="W89" s="51"/>
     </row>
-    <row r="90" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>612</v>
       </c>
@@ -17987,12 +17989,12 @@
       <c r="Q90" s="41">
         <v>1</v>
       </c>
-      <c r="V90" s="86" t="s">
+      <c r="V90" s="81" t="s">
         <v>652</v>
       </c>
-      <c r="W90" s="86"/>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W90" s="81"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>614</v>
       </c>
@@ -18012,7 +18014,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>616</v>
       </c>
@@ -18032,7 +18034,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>617</v>
       </c>
@@ -18052,7 +18054,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>618</v>
       </c>
@@ -18072,7 +18074,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>619</v>
       </c>
@@ -18086,7 +18088,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>621</v>
       </c>
@@ -18100,7 +18102,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>622</v>
       </c>
@@ -18114,7 +18116,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>623</v>
       </c>
@@ -18128,7 +18130,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V99" s="48">
         <v>45108</v>
       </c>
@@ -18136,7 +18138,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V100" s="48">
         <v>45352</v>
       </c>
@@ -18144,7 +18146,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V101" s="48">
         <v>45413</v>
       </c>
@@ -18152,7 +18154,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V102" s="48">
         <v>44986</v>
       </c>
@@ -18160,7 +18162,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V103" s="48">
         <v>44593</v>
       </c>
@@ -18168,7 +18170,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V104" s="48">
         <v>45017</v>
       </c>
@@ -18176,7 +18178,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V105" s="48">
         <v>44927</v>
       </c>
@@ -18184,7 +18186,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V106" s="48">
         <v>45170</v>
       </c>
@@ -18192,7 +18194,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V107" s="48">
         <v>44652</v>
       </c>
@@ -18200,7 +18202,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V108" s="48">
         <v>44348</v>
       </c>
@@ -18208,7 +18210,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V109" s="48">
         <v>45200</v>
       </c>
@@ -18216,7 +18218,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V110" s="48">
         <v>44621</v>
       </c>
@@ -18224,7 +18226,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V111" s="48">
         <v>45383</v>
       </c>
@@ -18232,7 +18234,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V112" s="48">
         <v>44075</v>
       </c>
@@ -18240,7 +18242,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="113" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V113" s="48">
         <v>44044</v>
       </c>
@@ -18248,7 +18250,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="114" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V114" s="48">
         <v>44562</v>
       </c>
@@ -18256,7 +18258,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="115" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V115" s="48">
         <v>45078</v>
       </c>
@@ -18264,7 +18266,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="116" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="116" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V116" s="48">
         <v>44958</v>
       </c>
@@ -18272,7 +18274,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="117" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V117" s="48">
         <v>45231</v>
       </c>
@@ -18280,7 +18282,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="118" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V118" s="48">
         <v>44440</v>
       </c>
@@ -18288,7 +18290,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="119" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V119" s="48">
         <v>44896</v>
       </c>
@@ -18296,7 +18298,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="120" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V120" s="48">
         <v>44835</v>
       </c>
@@ -18304,7 +18306,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="121" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V121" s="48">
         <v>44682</v>
       </c>
@@ -18312,7 +18314,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="122" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V122" s="48">
         <v>45444</v>
       </c>
@@ -18320,7 +18322,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="123" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V123" s="48">
         <v>44287</v>
       </c>
@@ -18328,7 +18330,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="124" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V124" s="48">
         <v>44774</v>
       </c>
@@ -18336,7 +18338,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="125" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V125" s="48">
         <v>43770</v>
       </c>
@@ -18344,7 +18346,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="126" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="126" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V126" s="48">
         <v>45597</v>
       </c>
@@ -18352,7 +18354,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="127" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="127" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V127" s="48">
         <v>45047</v>
       </c>
@@ -18360,7 +18362,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="128" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V128" s="48">
         <v>44805</v>
       </c>
@@ -18368,7 +18370,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="129" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V129" s="48">
         <v>44470</v>
       </c>
@@ -18376,7 +18378,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="130" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V130" s="48">
         <v>43831</v>
       </c>
@@ -18384,7 +18386,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="131" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V131" s="48">
         <v>44501</v>
       </c>
@@ -18392,7 +18394,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="132" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V132" s="48">
         <v>44228</v>
       </c>
@@ -18400,7 +18402,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="133" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V133" s="48">
         <v>43497</v>
       </c>
@@ -18408,7 +18410,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="134" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V134" s="48">
         <v>44378</v>
       </c>
@@ -18416,7 +18418,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="135" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V135" s="48">
         <v>44713</v>
       </c>
@@ -18424,7 +18426,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="136" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V136" s="48">
         <v>44743</v>
       </c>
@@ -18432,7 +18434,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="137" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V137" s="48">
         <v>45474</v>
       </c>
@@ -18440,7 +18442,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="138" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V138" s="48">
         <v>43862</v>
       </c>
@@ -18448,7 +18450,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="139" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V139" s="48">
         <v>44317</v>
       </c>
@@ -18461,12 +18463,20 @@
     <sortCondition descending="1" ref="K38:K55"/>
   </sortState>
   <mergeCells count="33">
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="V57:W57"/>
-    <mergeCell ref="V90:W90"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="S16:T16"/>
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="Y15:Z15"/>
@@ -18480,20 +18490,12 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="S2:T2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="V57:W57"/>
+    <mergeCell ref="V90:W90"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P62:Q62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -18507,30 +18509,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676618CE-DA8B-415A-9275-6758104F643B}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="90" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="G1" s="84" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="G1" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="84"/>
+      <c r="H1" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
ADD: Graph for Dates progression.
</commit_message>
<xml_diff>
--- a/datos_sms.xlsx
+++ b/datos_sms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\UNIR\Trabajo Fin de Master\Datos\qNLP-SMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A25ACF-9C4F-428A-B190-BDCAAA438656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF772598-C3E6-4898-BB44-A5B1677C70A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2562,7 +2562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2667,8 +2667,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2718,42 +2740,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2775,8 +2761,19 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3237,6 +3234,620 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Evolución</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> histórica</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Respuestas!$W$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Num</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Respuestas!$V$4:$V$54</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45323</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44866</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45413</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45444</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44835</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45292</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44896</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45474</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45505</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44317</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Respuestas!$W$4:$W$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-78AD-4D2C-ABE7-C9E35F5F97BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1461803792"/>
+        <c:axId val="1461810032"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1461803792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1461810032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1461810032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1461803792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5261,7 +5872,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Paises (Cómputo</a:t>
+              <a:t>Países (Cómputo</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -5634,7 +6245,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Paises (Proyectos </a:t>
+              <a:t>Países (Proyectos </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -6018,7 +6629,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Paises (Contribuciones académicas)</a:t>
+              <a:t>Países (Contribuciones académicas)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6325,6 +6936,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7171,6 +7822,522 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -11669,6 +12836,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>3726180</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3903A31E-CCE6-4E48-BEC4-00AD9479FFA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11937,7 +13142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -11949,30 +13154,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="61"/>
-      <c r="B2" s="70" t="s">
+      <c r="A2" s="69"/>
+      <c r="B2" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
       <c r="H2" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12047,12 +13252,12 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="59">
         <v>1393</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -12089,34 +13294,34 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="72" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="13"/>
       <c r="H12" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -12205,12 +13410,12 @@
       <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="59">
         <v>600</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>600</v>
@@ -12262,42 +13467,42 @@
       <c r="A20" s="16"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="17">
         <f>SUM(F14:F19)</f>
         <v>2803</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="78" t="s">
+      <c r="A23" s="75"/>
+      <c r="B23" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
       <c r="H23" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
+      <c r="A24" s="75"/>
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
@@ -12390,12 +13595,12 @@
       <c r="A28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="56">
+      <c r="B28" s="59">
         <v>65</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
       <c r="F28" s="21">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -12447,42 +13652,42 @@
       <c r="A31" s="16"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="79" t="s">
+      <c r="D31" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="79"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="22">
         <f>SUM(F25:F30)</f>
         <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="73"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="69"/>
-      <c r="B34" s="74" t="s">
+      <c r="A34" s="77"/>
+      <c r="B34" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
       <c r="H34" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="10" t="s">
         <v>0</v>
       </c>
@@ -12572,12 +13777,12 @@
       <c r="A39" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="56">
+      <c r="B39" s="59">
         <v>65</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="25">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -12626,10 +13831,10 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D42" s="71" t="s">
+      <c r="D42" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="E42" s="71"/>
+      <c r="E42" s="79"/>
       <c r="F42" s="26">
         <f>SUM(F36:F41)</f>
         <v>243</v>
@@ -12639,13 +13844,13 @@
       <c r="A44" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
       <c r="H44" s="29" t="s">
         <v>13</v>
       </c>
@@ -12654,15 +13859,15 @@
       <c r="A45" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65" t="s">
+      <c r="C45" s="73"/>
+      <c r="D45" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
       <c r="H45" s="4" t="s">
         <v>35</v>
       </c>
@@ -12671,30 +13876,22 @@
       <c r="A46" s="1">
         <v>112</v>
       </c>
-      <c r="B46" s="56">
+      <c r="B46" s="59">
         <v>48</v>
       </c>
-      <c r="C46" s="56"/>
-      <c r="D46" s="57">
+      <c r="C46" s="59"/>
+      <c r="D46" s="65">
         <f>SUM(A46:C46)</f>
         <v>160</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
       <c r="H46" s="4" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D31:E31"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D46:F46"/>
     <mergeCell ref="B1:E1"/>
@@ -12711,6 +13908,14 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17753,8 +18958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F3EEE0-596F-49A8-8C07-C0EC0504D81F}">
   <dimension ref="A1:Z139"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49"/>
+    <sheetView topLeftCell="H38" workbookViewId="0">
+      <selection activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17786,77 +18991,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="91" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="G1" s="83" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="G1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="83"/>
-      <c r="J1" s="84" t="s">
+      <c r="H1" s="92"/>
+      <c r="J1" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="M1" s="88" t="s">
+      <c r="K1" s="88"/>
+      <c r="M1" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="P1" s="89" t="s">
+      <c r="N1" s="84"/>
+      <c r="P1" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="V1" s="90" t="s">
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="V1" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="90"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="90" t="s">
         <v>581</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="D2" s="81" t="s">
+      <c r="B2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>628</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="G2" s="80" t="s">
+      <c r="E2" s="90"/>
+      <c r="G2" s="89" t="s">
         <v>581</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="J2" s="85" t="s">
+      <c r="H2" s="89"/>
+      <c r="J2" s="81" t="s">
         <v>581</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="M2" s="91" t="s">
+      <c r="K2" s="81"/>
+      <c r="M2" s="87" t="s">
         <v>581</v>
       </c>
-      <c r="N2" s="91"/>
-      <c r="P2" s="87" t="s">
+      <c r="N2" s="87"/>
+      <c r="P2" s="83" t="s">
         <v>581</v>
       </c>
-      <c r="Q2" s="87"/>
-      <c r="S2" s="87" t="s">
+      <c r="Q2" s="83"/>
+      <c r="S2" s="83" t="s">
         <v>628</v>
       </c>
-      <c r="T2" s="87"/>
-      <c r="V2" s="86" t="s">
+      <c r="T2" s="83"/>
+      <c r="V2" s="82" t="s">
         <v>581</v>
       </c>
-      <c r="W2" s="86"/>
-      <c r="Y2" s="86" t="s">
+      <c r="W2" s="82"/>
+      <c r="Y2" s="82" t="s">
         <v>628</v>
       </c>
-      <c r="Z2" s="86"/>
+      <c r="Z2" s="82"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
@@ -18323,7 +19528,7 @@
       <c r="E11" s="42">
         <v>5</v>
       </c>
-      <c r="G11" s="92"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="42"/>
       <c r="J11" s="52" t="s">
         <v>714</v>
@@ -18375,10 +19580,10 @@
       <c r="E12" s="42">
         <v>5</v>
       </c>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="89" t="s">
         <v>629</v>
       </c>
-      <c r="H12" s="80"/>
+      <c r="H12" s="89"/>
       <c r="J12" s="52" t="s">
         <v>658</v>
       </c>
@@ -18494,10 +19699,10 @@
       <c r="K14" s="41">
         <v>2</v>
       </c>
-      <c r="M14" s="91" t="s">
+      <c r="M14" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="91"/>
+      <c r="N14" s="87"/>
       <c r="P14" s="55" t="s">
         <v>686</v>
       </c>
@@ -18557,10 +19762,10 @@
       <c r="W15" s="42">
         <v>5</v>
       </c>
-      <c r="Y15" s="86" t="s">
+      <c r="Y15" s="82" t="s">
         <v>629</v>
       </c>
-      <c r="Z15" s="86"/>
+      <c r="Z15" s="82"/>
     </row>
     <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -18569,10 +19774,10 @@
       <c r="B16" s="43">
         <v>3</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="D16" s="90" t="s">
         <v>629</v>
       </c>
-      <c r="E16" s="81"/>
+      <c r="E16" s="90"/>
       <c r="G16" s="6" t="s">
         <v>645</v>
       </c>
@@ -18597,10 +19802,10 @@
       <c r="Q16" s="42">
         <v>3</v>
       </c>
-      <c r="S16" s="87" t="s">
+      <c r="S16" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="87"/>
+      <c r="T16" s="83"/>
       <c r="V16" s="48">
         <v>44958</v>
       </c>
@@ -18679,10 +19884,10 @@
       <c r="E18" s="42">
         <v>23</v>
       </c>
-      <c r="G18" s="80" t="s">
+      <c r="G18" s="89" t="s">
         <v>630</v>
       </c>
-      <c r="H18" s="80"/>
+      <c r="H18" s="89"/>
       <c r="J18" s="52" t="s">
         <v>663</v>
       </c>
@@ -18848,7 +20053,7 @@
       <c r="G21" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="H21" s="93">
+      <c r="H21" s="42">
         <v>9</v>
       </c>
       <c r="J21" s="52" t="s">
@@ -18900,7 +20105,7 @@
       <c r="G22" s="6" t="s">
         <v>643</v>
       </c>
-      <c r="H22" s="93">
+      <c r="H22" s="42">
         <v>3</v>
       </c>
       <c r="J22" s="52" t="s">
@@ -18909,10 +20114,10 @@
       <c r="K22" s="41">
         <v>1</v>
       </c>
-      <c r="M22" s="91" t="s">
+      <c r="M22" s="87" t="s">
         <v>582</v>
       </c>
-      <c r="N22" s="91"/>
+      <c r="N22" s="87"/>
       <c r="P22" s="55" t="s">
         <v>694</v>
       </c>
@@ -18954,7 +20159,7 @@
       <c r="G23" s="6" t="s">
         <v>644</v>
       </c>
-      <c r="H23" s="93">
+      <c r="H23" s="42">
         <v>2</v>
       </c>
       <c r="J23" s="52" t="s">
@@ -19007,7 +20212,7 @@
       <c r="E24" s="42">
         <v>1</v>
       </c>
-      <c r="G24" s="92"/>
+      <c r="G24" s="56"/>
       <c r="H24" s="42"/>
       <c r="J24" s="41"/>
       <c r="M24" s="53" t="s">
@@ -19054,10 +20259,10 @@
       <c r="E25" s="42">
         <v>1</v>
       </c>
-      <c r="J25" s="85" t="s">
+      <c r="J25" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="85"/>
+      <c r="K25" s="81"/>
       <c r="M25" s="53" t="s">
         <v>672</v>
       </c>
@@ -19227,10 +20432,10 @@
       <c r="W28" s="42">
         <v>3</v>
       </c>
-      <c r="Y28" s="86" t="s">
+      <c r="Y28" s="82" t="s">
         <v>651</v>
       </c>
-      <c r="Z28" s="86"/>
+      <c r="Z28" s="82"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -19281,10 +20486,10 @@
       <c r="B30" s="43">
         <v>1</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="90" t="s">
         <v>630</v>
       </c>
-      <c r="E30" s="81"/>
+      <c r="E30" s="90"/>
       <c r="J30" s="52" t="s">
         <v>657</v>
       </c>
@@ -19303,10 +20508,10 @@
       <c r="Q30" s="42">
         <v>1</v>
       </c>
-      <c r="S30" s="87" t="s">
+      <c r="S30" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="T30" s="87"/>
+      <c r="T30" s="83"/>
       <c r="V30" s="48">
         <v>44774</v>
       </c>
@@ -19549,10 +20754,10 @@
       <c r="E36" s="43">
         <v>6</v>
       </c>
-      <c r="J36" s="85" t="s">
+      <c r="J36" s="81" t="s">
         <v>582</v>
       </c>
-      <c r="K36" s="85"/>
+      <c r="K36" s="81"/>
       <c r="P36" s="55" t="s">
         <v>709</v>
       </c>
@@ -19767,10 +20972,10 @@
       <c r="K41" s="41">
         <v>4</v>
       </c>
-      <c r="P41" s="87" t="s">
+      <c r="P41" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="Q41" s="87"/>
+      <c r="Q41" s="83"/>
       <c r="S41" s="55" t="s">
         <v>693</v>
       </c>
@@ -19899,10 +21104,10 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="81"/>
+      <c r="B46" s="90"/>
       <c r="J46" s="52" t="s">
         <v>657</v>
       </c>
@@ -20184,10 +21389,10 @@
       <c r="Q57" s="42">
         <v>1</v>
       </c>
-      <c r="V57" s="86" t="s">
+      <c r="V57" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="W57" s="86"/>
+      <c r="W57" s="82"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
@@ -20224,10 +21429,10 @@
       </c>
     </row>
     <row r="60" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="90" t="s">
         <v>582</v>
       </c>
-      <c r="B60" s="81"/>
+      <c r="B60" s="90"/>
       <c r="P60" s="54" t="s">
         <v>703</v>
       </c>
@@ -20264,10 +21469,10 @@
       <c r="B62" s="43">
         <v>43</v>
       </c>
-      <c r="P62" s="87" t="s">
+      <c r="P62" s="83" t="s">
         <v>582</v>
       </c>
-      <c r="Q62" s="87"/>
+      <c r="Q62" s="83"/>
       <c r="V62" s="48">
         <v>45231</v>
       </c>
@@ -20824,10 +22029,10 @@
       <c r="Q90" s="41">
         <v>1</v>
       </c>
-      <c r="V90" s="86" t="s">
+      <c r="V90" s="82" t="s">
         <v>650</v>
       </c>
-      <c r="W90" s="86"/>
+      <c r="W90" s="82"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
@@ -21298,12 +22503,20 @@
     <sortCondition descending="1" ref="K38:K55"/>
   </sortState>
   <mergeCells count="33">
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="V57:W57"/>
-    <mergeCell ref="V90:W90"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="S16:T16"/>
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="Y15:Z15"/>
@@ -21317,20 +22530,12 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="S2:T2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="V57:W57"/>
+    <mergeCell ref="V90:W90"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P62:Q62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -21344,8 +22549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676618CE-DA8B-415A-9275-6758104F643B}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21357,34 +22562,35 @@
     <col min="9" max="9" width="3.33203125" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" customWidth="1"/>
     <col min="15" max="15" width="3.33203125" customWidth="1"/>
+    <col min="20" max="20" width="54.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="91" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="G1" s="84" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="G1" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="J1" s="89" t="s">
+      <c r="H1" s="88"/>
+      <c r="J1" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="P1" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>